<commit_message>
Docs: Finish up website test docs
</commit_message>
<xml_diff>
--- a/docs/Website Tests.xlsx
+++ b/docs/Website Tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="118">
   <si>
     <t xml:space="preserve">Projekt Neve:</t>
   </si>
@@ -99,24 +99,8 @@
 Navigációs sávban.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Következő URL megnyitása:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">http://localhost:8080</t>
-    </r>
+    <t xml:space="preserve">Következő URL megnyitása:
+http://localhost:8080</t>
   </si>
   <si>
     <t xml:space="preserve">A kosarad üres felület megjelenése</t>
@@ -145,7 +129,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Név: Teszt Név
+      <t xml:space="preserve">Név: Teszt Név 
 Email: </t>
     </r>
     <r>
@@ -195,9 +179,8 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Név: Teszt Bob
+      <t xml:space="preserve">Név: Teszt Bob 
 Email: </t>
     </r>
     <r>
@@ -206,19 +189,17 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">tesztbob@example</t>
+      <t xml:space="preserve">tesztbob@example.hu
+</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">.hu
-Telefonszám: 321321321</t>
+      <t xml:space="preserve">Telefonszám: 321321321</t>
     </r>
   </si>
   <si>
@@ -238,36 +219,9 @@
 5. „Rendelés Küldése” gomb megnyomása</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Név: Teszt
-Email: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">nev@example.com
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Telefonszám: 9876543210</t>
-    </r>
+    <t xml:space="preserve">Név: Teszt 
+Email: nev@example.com 
+Telefonszám: 9876543210</t>
   </si>
   <si>
     <t xml:space="preserve">TE_005</t>
@@ -300,36 +254,9 @@
 Megadása</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Név: Teszt Bob
-Email: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">tesztbob@example</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.hu
+    <t xml:space="preserve">Név: Teszt Bob 
+Email: tesztbob@example.hu 
 Telefonszám: 123456789</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">TE_007</t>
@@ -339,36 +266,9 @@
 Helyes Email Telefonszám Megadása</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Név: 
-Email: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">nev@example.com
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Telefonszám: 123123123</t>
-    </r>
+    <t xml:space="preserve">Név:  
+Email: nev@example.com 
+Telefonszám: 123123123</t>
   </si>
   <si>
     <t xml:space="preserve">„Please fill out this field” validáció
@@ -379,33 +279,8 @@
     <t xml:space="preserve">TE_008</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Helyes Név, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Telefonszám 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Helytelen Email Megadása</t>
-    </r>
+    <t xml:space="preserve">Helyes Név, Telefonszám 
+Helytelen Email Megadása</t>
   </si>
   <si>
     <t xml:space="preserve">Név: Bob
@@ -416,33 +291,8 @@
     <t xml:space="preserve">TE_009</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Helyes Név, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Telefonszám 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Üres Email Megadása</t>
-    </r>
+    <t xml:space="preserve">Helyes Név, Telefonszám 
+Üres Email Megadása</t>
   </si>
   <si>
     <t xml:space="preserve">Név: Bob
@@ -453,50 +303,8 @@
     <t xml:space="preserve">TE_010</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Helyes Név, Email</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Üres </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Telefonszám</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Megadása</t>
-    </r>
+    <t xml:space="preserve">Helyes Név, Email 
+Üres Telefonszám Megadása</t>
   </si>
   <si>
     <t xml:space="preserve">Név: Bob
@@ -517,39 +325,14 @@
     <t xml:space="preserve">Ételek hozzáadása és kivétele</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
 Sávban.
 2. Három ételből három darab kosárba helyezése a
 „Kosárba” gomb megnyomásával
 3. Kosár gomb megnyomása navigációs
 Sávban.
-4. Első </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">étel kivétele a törlés gomb megnyomásával
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">5. Utolsó étel kivétele a törlés gomb megnyomásával</t>
-    </r>
+4. Első étel kivétele a törlés gomb megnyomásával
+5. Utolsó étel kivétele a törlés gomb megnyomásával</t>
   </si>
   <si>
     <t xml:space="preserve">A kiválasztott ételek kivétele
@@ -589,6 +372,72 @@
   </si>
   <si>
     <t xml:space="preserve">Jelszó: asd123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Következő URL megnyitása:
+http://localhost:8080/admin
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin felület megjelenése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helytelen jelszó</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jelszó: qwe321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">„Sikertelen bejelentkezés” szöveg megjelenése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Üresen hagyott jelszó</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jelszó: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">„Please fill out this field” validáció
+szöveg megjelenése a jelszó
+Beviteli mezőn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH_WE_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rendelések státuszának változtatása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rendelés kész státusz beállítása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
+Sávban.
+2. Egy étel kosárhoz adása a
+„Kosárba” gomb megnyomásával
+3. Kosár gomb megnyomása navigációs
+Sávban.
+4. Rendelési adatok kitöltése
+5. „Rendelés Küldése” gomb megnyomása
+6. /admin URL megnyitása
+7. Jelszó beírása
+8. A beküldött rendelésnél a Kész gomb
+Megnyomása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Név: Teszt Bob
+Email: tesztbob@example.hu
+Telefonszám: 321321321
+Jelszó: asd123</t>
   </si>
   <si>
     <r>
@@ -609,60 +458,21 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">http://localhost:8080/admin
-</t>
+      <t xml:space="preserve">http://localhost:8080</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Admin felület megjelenése</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helytelen jelszó</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jelszó: qwe321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">„Sikertelen bejelentkezés” szöveg megjelenése</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE_015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Üresen hagyott jelszó</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jelszó: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">„Please fill out this field” validáció
-szöveg megjelenése a jelszó
-Beviteli mezőn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TH_WE_005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rendelések státuszának változtatása</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE_016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rendelés kész státusz beállítása</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
+    <t xml:space="preserve">A beküldött rendelés státusza
+Elkészültre változott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE_017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rendelés visszavonása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
 Sávban.
 2. Egy étel kosárhoz adása a
 „Kosárba” gomb megnyomásával
@@ -672,15 +482,48 @@
 5. „Rendelés Küldése” gomb megnyomása
 6. /admin URL megnyitása
 7. Jelszó beírása
-8. A </t>
-    </r>
+8. A beküldött rendelésnél a „Kész” gomb
+Megnyomása
+9. Korábbi rendelések megjelenítése gomb
+Megnyomása
+10. A beküldött rendelésnél a „Visszavon” gomb
+Megnyomása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A beküldött rendelés a jelenlegi 
+Rendelések közé került változott</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH_WE_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ételek szerkesztésének ellenőrzése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE_018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Új étel hozzá adása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. /admin URL megnyitása
+2. Jelszó beírása
+3. A Ételek szerkesztésének megjelenítése gomb
+Megnyomása
+4. Új Étel hozzáadása gomb megnyomása
+5. Étel adatainak kitöltése
+6. Étel feltöltése gomb megnyomása
+7. Biztosan feltöltöd elfogadása</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">beküldött</t>
+      <t xml:space="preserve">Jelszó: asd123
+</t>
     </r>
     <r>
       <rPr>
@@ -689,49 +532,86 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> rendelésnél a Kész gomb
-Megnyomása</t>
+      <t xml:space="preserve">Név: Teszt Étel
+Leírás: A legfinomabb teszt étel
+Kép útvonal: Somloi-galuska-scaled.jpg
+Ár: 850</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Név: Teszt Bob
-Email: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">tesztbob@example</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.hu
-Telefonszám: 321321321
-Jelszó: asd123</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">A beküldött rendelés státusza
-Elkészültre változott</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE_017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rendelés visszavonása</t>
+    <t xml:space="preserve">Feltöltött étel megjelenése az ételek
+Listában</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE_019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Étel módosítása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. /admin URL megnyitása
+2. Jelszó beírása
+3. A Ételek szerkesztésének megjelenítése gomb
+Megnyomása
+4. Első ételnél a módosítás gomb megnyomása
+5. Étel adatainak kitöltése
+6. Étel feltöltése gomb megnyomása
+7. Biztosan feltöltöd elfogadása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feltöltött étel adatainak megjelenése a
+ételek listában</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE_020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Étel sikeres törlése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. /admin URL megnyitása
+2. Jelszó beírása
+3. A Ételek szerkesztésének megjelenítése gomb
+Megnyomása
+4. Új Étel hozzáadása gomb megnyomása
+5. Étel adatainak kitöltése
+6. Étel feltöltése gomb megnyomása
+7. Biztosan feltöltöd elfogadása
+8. A feltöltött étel kikeresése
+9. A feltöltött ételnél a törlés gomb megnyomása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feltöltött étel törlődése az ételek
+Listából</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE_021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Étel sikertelen törlése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. /admin URL megnyitása
+2. Jelszó beírása
+3. A Ételek szerkesztésének megjelenítése gomb
+Megnyomása
+4. Új Étel hozzáadása gomb megnyomása
+5. Étel adatainak kitöltése
+6. Étel feltöltése gomb megnyomása
+7. Biztosan feltöltöd elfogadása
+8. Ételek gombra kattintás a navigációs
+Sávban.
+9. Egy étel kosárhoz adása a
+„Kosárba” gomb megnyomásával
+10. Kosár gomb megnyomása navigációs
+Sávban.
+11. Rendelési adatok kitöltése
+12. „Rendelés Küldése” gomb megnyomása
+13. /admin URL megnyitása
+14. A feltöltött étel kikeresése
+15. A Ételek szerkesztésének megjelenítése gomb
+16. A feltöltött ételnél a törlés gomb megnyomása
+17. Biztosan törlöd elfogadása.</t>
   </si>
   <si>
     <r>
@@ -741,25 +621,19 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
-2. Egy étel kosárhoz adása a
-„Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
-4. Rendelési adatok kitöltése
-5. „Rendelés Küldése” gomb megnyomása
-6. /admin URL megnyitása
-7. Jelszó beírása
-8. A </t>
+      <t xml:space="preserve">Jelszó: asd123
+</t>
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">beküldött</t>
+      <t xml:space="preserve">Étel adatai:
+</t>
     </r>
     <r>
       <rPr>
@@ -768,11 +642,22 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> rendelésnél a „Kész” gomb
-Megnyomása
-9. Korábbi rendelések megjelenítése gomb
-Megnyomása
-10. </t>
+      <t xml:space="preserve">Név: Teszt Étel
+Leírás: A legfinomabb teszt étel
+Kép útvonal: Somloi-galuska-scaled.jpg
+Ár: 850
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rendelés adatai:
+</t>
     </r>
     <r>
       <rPr>
@@ -780,13 +665,13 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">A beküldött rendelésnél a „Visszavon” gomb
-Megnyomása</t>
+      <t xml:space="preserve">Név: Teszt Bob 
+Email: tesztbob@example.hu 
+Telefonszám: 123456789</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">A beküldött rendelés a jelenlegi 
-Rendelések közé került változott</t>
+    <t xml:space="preserve">Sikertelen törlés alert megjelenése</t>
   </si>
 </sst>
 </file>
@@ -798,7 +683,7 @@
     <numFmt numFmtId="165" formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="\$#,##0_);[RED]&quot;($&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -839,6 +724,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -849,8 +741,8 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1077,7 +969,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1090,8 +982,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1106,19 +998,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1126,23 +1018,47 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1150,72 +1066,8 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1414,10 +1266,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1427,12 +1279,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="44.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="27.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="21.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,18 +1299,18 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -1524,16 +1376,16 @@
         <v>24</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="12" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
-      <c r="L7" s="14"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="140.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1542,23 +1394,23 @@
       <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="6" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="13"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
-      <c r="L8" s="14"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="122.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1567,21 +1419,21 @@
       <c r="C9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="20"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
       <c r="M9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="119.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1590,17 +1442,17 @@
       <c r="C10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -1612,41 +1464,41 @@
       <c r="C11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" s="23" customFormat="true" ht="142.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" s="18" customFormat="true" ht="142.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="17"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -1654,21 +1506,21 @@
     </row>
     <row r="13" customFormat="false" ht="132.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="24" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="21" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="12" t="s">
         <v>51</v>
       </c>
       <c r="I13" s="13"/>
@@ -1678,20 +1530,20 @@
     </row>
     <row r="14" customFormat="false" ht="118" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="24" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="12"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="12"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
@@ -1700,20 +1552,20 @@
     </row>
     <row r="15" customFormat="false" ht="118" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="24" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="12"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
@@ -1722,20 +1574,20 @@
     </row>
     <row r="16" customFormat="false" ht="130.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="24" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="12"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
@@ -1743,24 +1595,24 @@
       <c r="L16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="115.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="21" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="12" t="s">
         <v>66</v>
       </c>
       <c r="I17" s="13"/>
@@ -1769,20 +1621,20 @@
       <c r="L17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="115.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="26" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I18" s="13"/>
@@ -1797,66 +1649,66 @@
       <c r="B19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="55.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="28" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="30" t="s">
+      <c r="G20" s="14"/>
+      <c r="H20" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="33.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="15" t="s">
+      <c r="E21" s="12"/>
+      <c r="F21" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16" t="s">
+      <c r="G21" s="14"/>
+      <c r="H21" s="12" t="s">
         <v>85</v>
       </c>
       <c r="I21" s="10"/>
@@ -1865,29 +1717,29 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="164.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="14" t="s">
         <v>90</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="30" t="s">
+      <c r="G22" s="7" t="s">
         <v>92</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -1895,46 +1747,151 @@
       <c r="L22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="198.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="26" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="D23" s="9" t="s">
         <v>95</v>
       </c>
+      <c r="E23" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="30" t="s">
-        <v>96</v>
+      <c r="G23" s="7"/>
+      <c r="H23" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="0"/>
-      <c r="F24" s="0"/>
-      <c r="G24" s="0"/>
-      <c r="H24" s="0"/>
-      <c r="I24" s="0"/>
-      <c r="J24" s="0"/>
-      <c r="K24" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="0"/>
-      <c r="G27" s="34"/>
+    <row r="24" customFormat="false" ht="114.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="16"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+    </row>
+    <row r="27" customFormat="false" ht="309.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F28" s="3"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F30" s="24"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="24"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F34" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="22">
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="G7:G18"/>
@@ -1953,17 +1910,16 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="F22:F23"/>
     <mergeCell ref="G22:G23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="G24:G26"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" display="http://localhost:8080"/>
-    <hyperlink ref="F8" r:id="rId2" display="nev@example.com"/>
-    <hyperlink ref="F9" r:id="rId3" display="tesztbob@example"/>
-    <hyperlink ref="F10" r:id="rId4" display="nev@example.com"/>
-    <hyperlink ref="F12" r:id="rId5" display="tesztbob@example"/>
-    <hyperlink ref="F13" r:id="rId6" display="nev@example.com"/>
-    <hyperlink ref="G19" r:id="rId7" display="http://localhost:8080/admin"/>
-    <hyperlink ref="F22" r:id="rId8" display="tesztbob@example"/>
-    <hyperlink ref="G22" r:id="rId9" display="http://localhost:8080"/>
+    <hyperlink ref="F8" r:id="rId1" display="nev@example.com"/>
+    <hyperlink ref="F9" r:id="rId2" display="tesztbob@example.hu"/>
+    <hyperlink ref="G22" r:id="rId3" display="http://localhost:8080"/>
+    <hyperlink ref="G27" r:id="rId4" display="http://localhost:8080"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Docs: Format documents, update table of contents
</commit_message>
<xml_diff>
--- a/docs/Website Tests.xlsx
+++ b/docs/Website Tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
   <si>
     <t xml:space="preserve">Projekt Neve:</t>
   </si>
@@ -122,36 +122,9 @@
 5. „Rendelés Küldése” gomb megnyomása</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Név: Teszt Név 
-Email: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">nev@example.com
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Telefonszám: 123123123</t>
-    </r>
+    <t xml:space="preserve">Név: Teszt Név 
+Email: nev@example.com
+Telefonszám: 123123123</t>
   </si>
   <si>
     <t xml:space="preserve">Sikeres beküldés alert megjelenése</t>
@@ -174,33 +147,9 @@
 5. „Rendelés Küldése” gomb megnyomása</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Név: Teszt Bob 
-Email: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">tesztbob@example.hu
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Telefonszám: 321321321</t>
-    </r>
+    <t xml:space="preserve">Név: Teszt Bob 
+Email: tesztbob@example.hu
+Telefonszám: 321321321</t>
   </si>
   <si>
     <t xml:space="preserve">TE_004</t>
@@ -438,28 +387,6 @@
 Email: tesztbob@example.hu
 Telefonszám: 321321321
 Jelszó: asd123</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Következő URL megnyitása:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://localhost:8080</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">A beküldött rendelés státusza
@@ -516,27 +443,11 @@
 7. Biztosan feltöltöd elfogadása</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Jelszó: asd123
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Név: Teszt Étel
+    <t xml:space="preserve">Jelszó: asd123
+Név: Teszt Étel
 Leírás: A legfinomabb teszt étel
 Kép útvonal: Somloi-galuska-scaled.jpg
 Ár: 850</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Feltöltött étel megjelenése az ételek
@@ -664,6 +575,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Név: Teszt Bob 
 Email: tesztbob@example.hu 
@@ -683,7 +595,7 @@
     <numFmt numFmtId="165" formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="\$#,##0_);[RED]&quot;($&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -728,17 +640,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -969,7 +870,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1030,11 +931,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1054,12 +951,8 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1268,8 +1161,8 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1400,14 +1293,14 @@
       <c r="E8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="15" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="15"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -1425,7 +1318,7 @@
       <c r="E9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="7"/>
@@ -1478,7 +1371,7 @@
       <c r="K11" s="13"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" s="18" customFormat="true" ht="142.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" s="17" customFormat="true" ht="142.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>43</v>
       </c>
@@ -1498,7 +1391,7 @@
         <v>47</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="17"/>
+      <c r="H12" s="16"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -1507,7 +1400,7 @@
     <row r="13" customFormat="false" ht="132.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -1531,7 +1424,7 @@
     <row r="14" customFormat="false" ht="118" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="12" t="s">
@@ -1553,7 +1446,7 @@
     <row r="15" customFormat="false" ht="118" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>55</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -1575,7 +1468,7 @@
     <row r="16" customFormat="false" ht="130.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="18" t="s">
         <v>58</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -1667,15 +1560,15 @@
       <c r="H19" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="55.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -1697,7 +1590,7 @@
     <row r="21" customFormat="false" ht="33.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>82</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -1735,11 +1628,11 @@
       <c r="F22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>92</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
@@ -1750,18 +1643,18 @@
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
@@ -1770,28 +1663,28 @@
     </row>
     <row r="24" customFormat="false" ht="114.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="E24" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="F24" s="21" t="s">
         <v>102</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H24" s="16" t="s">
-        <v>104</v>
+      <c r="H24" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
@@ -1802,18 +1695,18 @@
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="E25" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="F25" s="21"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="21" t="s">
-        <v>108</v>
       </c>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1824,18 +1717,18 @@
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="E26" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="F26" s="16"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="7"/>
       <c r="H26" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
@@ -1845,23 +1738,23 @@
     <row r="27" customFormat="false" ht="309.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="E27" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="F27" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="G27" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
@@ -1870,25 +1763,25 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F28" s="3"/>
-      <c r="G28" s="18"/>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="24"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="24"/>
+      <c r="F31" s="22"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="24"/>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="24"/>
+      <c r="F33" s="22"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="24"/>
+      <c r="F34" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -1916,10 +1809,10 @@
     <mergeCell ref="G24:G26"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="nev@example.com"/>
-    <hyperlink ref="F9" r:id="rId2" display="tesztbob@example.hu"/>
-    <hyperlink ref="G22" r:id="rId3" display="http://localhost:8080"/>
-    <hyperlink ref="G27" r:id="rId4" display="http://localhost:8080"/>
+    <hyperlink ref="F8" r:id="rId1" display="Név: Teszt Név &#10;Email: nev@example.com&#10;Telefonszám: 123123123"/>
+    <hyperlink ref="F9" r:id="rId2" display="Név: Teszt Bob &#10;Email: tesztbob@example.hu&#10;Telefonszám: 321321321"/>
+    <hyperlink ref="G22" r:id="rId3" display="Következő URL megnyitása:&#10;http://localhost:8080"/>
+    <hyperlink ref="G27" r:id="rId4" display="Következő URL megnyitása:&#10;http://localhost:8080"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Test: Finish up website test docs, export to pdf
</commit_message>
<xml_diff>
--- a/docs/Website Tests.xlsx
+++ b/docs/Website Tests.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Teszt esetek" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Teszt esetek'!$A$1:$L$27</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
   <si>
     <t xml:space="preserve">Projekt Neve:</t>
   </si>
@@ -28,31 +31,85 @@
     <t xml:space="preserve">etlap</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Színkódok:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zöld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piros</t>
+  </si>
+  <si>
     <t xml:space="preserve">Modul Neve:</t>
   </si>
   <si>
     <t xml:space="preserve">website-etlap</t>
   </si>
   <si>
+    <t xml:space="preserve">Teszt eset ID:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sikeres út</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hibás út</t>
+  </si>
+  <si>
     <t xml:space="preserve">Készítette:</t>
   </si>
   <si>
-    <t xml:space="preserve">Surmann Márk</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Buda Levente István
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ócsai Márk
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Surmann Márk</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass/Fail:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sikeres teszt eredmény</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sikertelen teszt eredmény</t>
   </si>
   <si>
     <t xml:space="preserve">Készítés ideje:</t>
   </si>
   <si>
-    <t xml:space="preserve">2025.03.15</t>
+    <t xml:space="preserve">2025.03.19</t>
   </si>
   <si>
     <t xml:space="preserve">Teszthelyzet ID:</t>
   </si>
   <si>
     <t xml:space="preserve">Teszthelyzet leírás:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teszt eset ID:</t>
   </si>
   <si>
     <t xml:space="preserve">Teszteset leírás:</t>
@@ -92,11 +149,10 @@
     <t xml:space="preserve">TE_001</t>
   </si>
   <si>
-    <t xml:space="preserve">Üres kosár megjelenésé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Kosár gombra kattintás a
-Navigációs sávban.</t>
+    <t xml:space="preserve">Üres kosár megjelenése</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Kosár gombra kattintás a navigációs sávban.</t>
   </si>
   <si>
     <t xml:space="preserve">Következő URL megnyitása:
@@ -106,18 +162,25 @@
     <t xml:space="preserve">A kosarad üres felület megjelenése</t>
   </si>
   <si>
+    <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surmann Márk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025.03.18</t>
+  </si>
+  <si>
     <t xml:space="preserve">TE_002</t>
   </si>
   <si>
     <t xml:space="preserve">Egy étel kosárba helyezése</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs sávban.
 2. Egy étel kosárhoz adása a
 „Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
+3. Kosár gomb megnyomása navigációs sávban.
 4. Rendelési adatok kitöltése
 5. „Rendelés Küldése” gomb megnyomása</t>
   </si>
@@ -137,12 +200,10 @@
 1 darab</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs sávban.
 2. Két étel kosárhoz adása a
 „Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
+3. Kosár gomb megnyomása navigációs sávban.
 4. Rendelési adatok kitöltése
 5. „Rendelés Küldése” gomb megnyomása</t>
   </si>
@@ -152,18 +213,19 @@
 Telefonszám: 321321321</t>
   </si>
   <si>
+    <t xml:space="preserve">Buda Levente István</t>
+  </si>
+  <si>
     <t xml:space="preserve">TE_004</t>
   </si>
   <si>
     <t xml:space="preserve">Egy ételből több kosárba helyezése</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs sávban.
 2. Egy ételből három kosárba helyezése a
 „Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
+3. Kosár gomb megnyomása navigációs sávban.
 4. Rendelési adatok kitöltése
 5. „Rendelés Küldése” gomb megnyomása</t>
   </si>
@@ -179,12 +241,10 @@
     <t xml:space="preserve">Több ételből több kosárba helyezése</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs sávban.
 2. Három ételből három darab kosárba helyezése a
 „Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
+3. Kosár gomb megnyomása navigációs sávban.
 4. Rendelési adatok kitöltése
 5. „Rendelés Küldése” gomb megnyomása</t>
   </si>
@@ -192,15 +252,13 @@
     <t xml:space="preserve">TH_WE_002</t>
   </si>
   <si>
-    <t xml:space="preserve">Rendelési adatok
-Megadása</t>
+    <t xml:space="preserve">Rendelési adatok megadása</t>
   </si>
   <si>
     <t xml:space="preserve">TE_006</t>
   </si>
   <si>
-    <t xml:space="preserve">Helyes Név, Email, Telefonszám
-Megadása</t>
+    <t xml:space="preserve">Helyes Név, Email, Telefonszám megadása</t>
   </si>
   <si>
     <t xml:space="preserve">Név: Teszt Bob 
@@ -212,7 +270,7 @@
   </si>
   <si>
     <t xml:space="preserve">Üres Név
-Helyes Email Telefonszám Megadása</t>
+Helyes Email, Telefonszám megadása</t>
   </si>
   <si>
     <t xml:space="preserve">Név:  
@@ -221,15 +279,14 @@
   </si>
   <si>
     <t xml:space="preserve">„Please fill out this field” validáció
-szöveg megjelenése a
-Beviteli mezőn</t>
+szöveg megjelenése a beviteli mezőn</t>
   </si>
   <si>
     <t xml:space="preserve">TE_008</t>
   </si>
   <si>
     <t xml:space="preserve">Helyes Név, Telefonszám 
-Helytelen Email Megadása</t>
+Helytelen Email megadása</t>
   </si>
   <si>
     <t xml:space="preserve">Név: Bob
@@ -237,11 +294,14 @@
 Telefonszám: 123123123</t>
   </si>
   <si>
+    <t xml:space="preserve">Ócsai Márk</t>
+  </si>
+  <si>
     <t xml:space="preserve">TE_009</t>
   </si>
   <si>
     <t xml:space="preserve">Helyes Név, Telefonszám 
-Üres Email Megadása</t>
+Üres Email megadása</t>
   </si>
   <si>
     <t xml:space="preserve">Név: Bob
@@ -252,8 +312,8 @@
     <t xml:space="preserve">TE_010</t>
   </si>
   <si>
-    <t xml:space="preserve">Helyes Név, Email 
-Üres Telefonszám Megadása</t>
+    <t xml:space="preserve">Helyes Név, Email  
+Üres Telefonszám megadása</t>
   </si>
   <si>
     <t xml:space="preserve">Név: Bob
@@ -264,8 +324,7 @@
     <t xml:space="preserve">TH_WE_003</t>
   </si>
   <si>
-    <t xml:space="preserve">Ételek hozzáadása és törlése
- A kosárból</t>
+    <t xml:space="preserve">Ételek hozzáadása és törlése a kosárból</t>
   </si>
   <si>
     <t xml:space="preserve">TE_011</t>
@@ -274,18 +333,15 @@
     <t xml:space="preserve">Ételek hozzáadása és kivétele</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs sávban.
 2. Három ételből három darab kosárba helyezése a
 „Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
+3. Kosár gomb megnyomása navigációs sávban.
 4. Első étel kivétele a törlés gomb megnyomásával
 5. Utolsó étel kivétele a törlés gomb megnyomásával</t>
   </si>
   <si>
-    <t xml:space="preserve">A kiválasztott ételek kivétele
-A kosárból</t>
+    <t xml:space="preserve">A kiválasztott ételek kivétele a kosárból</t>
   </si>
   <si>
     <t xml:space="preserve">TE_012</t>
@@ -294,20 +350,17 @@
     <t xml:space="preserve">Kosár kiürítése gomb</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs sávban.
 2. Három ételből három darab kosárba helyezése a
 „Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
+3. Kosár gomb megnyomása navigációs sávban.
 4. Kosár kiürítése gomb megnyomása</t>
   </si>
   <si>
     <t xml:space="preserve">TH_WE_004</t>
   </si>
   <si>
-    <t xml:space="preserve">Admin Bejelentkezés 
-Funkció ellenőrzése</t>
+    <t xml:space="preserve">Admin Bejelentkezés funkció ellenőrzése</t>
   </si>
   <si>
     <t xml:space="preserve">TE_013</t>
@@ -353,8 +406,7 @@
   </si>
   <si>
     <t xml:space="preserve">„Please fill out this field” validáció
-szöveg megjelenése a jelszó
-Beviteli mezőn</t>
+szöveg megjelenése a jelszó beviteli mezőn</t>
   </si>
   <si>
     <t xml:space="preserve">TH_WE_005</t>
@@ -369,18 +421,15 @@
     <t xml:space="preserve">Rendelés kész státusz beállítása</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs sávban.
 2. Egy étel kosárhoz adása a
 „Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
+3. Kosár gomb megnyomása navigációs sávban.
 4. Rendelési adatok kitöltése
 5. „Rendelés Küldése” gomb megnyomása
 6. /admin URL megnyitása
 7. Jelszó beírása
-8. A beküldött rendelésnél a Kész gomb
-Megnyomása</t>
+8. A beküldött rendelésnél a Kész gomb megnyomása</t>
   </si>
   <si>
     <t xml:space="preserve">Név: Teszt Bob
@@ -389,8 +438,7 @@
 Jelszó: asd123</t>
   </si>
   <si>
-    <t xml:space="preserve">A beküldött rendelés státusza
-Elkészültre változott</t>
+    <t xml:space="preserve">A beküldött rendelés státusza elkészültre változott</t>
   </si>
   <si>
     <t xml:space="preserve">TE_017</t>
@@ -399,26 +447,20 @@
     <t xml:space="preserve">Rendelés visszavonása</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs
-Sávban.
+    <t xml:space="preserve">1. Ételek gombra kattintás a navigációs sávban.
 2. Egy étel kosárhoz adása a
 „Kosárba” gomb megnyomásával
-3. Kosár gomb megnyomása navigációs
-Sávban.
+3. Kosár gomb megnyomása navigációs sávban.
 4. Rendelési adatok kitöltése
 5. „Rendelés Küldése” gomb megnyomása
 6. /admin URL megnyitása
 7. Jelszó beírása
-8. A beküldött rendelésnél a „Kész” gomb
-Megnyomása
-9. Korábbi rendelések megjelenítése gomb
-Megnyomása
-10. A beküldött rendelésnél a „Visszavon” gomb
-Megnyomása</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A beküldött rendelés a jelenlegi 
-Rendelések közé került változott</t>
+8. A beküldött rendelésnél a „Kész” gomb megnyomása
+9. Korábbi rendelések megjelenítése gomb megnyomása
+10. A beküldött rendelésnél a „Visszavon” gomb megnyomása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A beküldött rendelés a jelenlegi rendelések közé került változott</t>
   </si>
   <si>
     <t xml:space="preserve">TH_WE_006</t>
@@ -450,8 +492,7 @@
 Ár: 850</t>
   </si>
   <si>
-    <t xml:space="preserve">Feltöltött étel megjelenése az ételek
-Listában</t>
+    <t xml:space="preserve">Feltöltött étel megjelenése az ételek listában</t>
   </si>
   <si>
     <t xml:space="preserve">TE_019</t>
@@ -462,8 +503,7 @@
   <si>
     <t xml:space="preserve">1. /admin URL megnyitása
 2. Jelszó beírása
-3. A Ételek szerkesztésének megjelenítése gomb
-Megnyomása
+3. Az Ételek szerkesztésének megjelenítése gomb megnyomása
 4. Első ételnél a módosítás gomb megnyomása
 5. Étel adatainak kitöltése
 6. Étel feltöltése gomb megnyomása
@@ -482,8 +522,7 @@
   <si>
     <t xml:space="preserve">1. /admin URL megnyitása
 2. Jelszó beírása
-3. A Ételek szerkesztésének megjelenítése gomb
-Megnyomása
+3. Az Ételek szerkesztésének megjelenítése gomb megnyomása
 4. Új Étel hozzáadása gomb megnyomása
 5. Étel adatainak kitöltése
 6. Étel feltöltése gomb megnyomása
@@ -492,8 +531,7 @@
 9. A feltöltött ételnél a törlés gomb megnyomása</t>
   </si>
   <si>
-    <t xml:space="preserve">Feltöltött étel törlődése az ételek
-Listából</t>
+    <t xml:space="preserve">Feltöltött étel törlődése az ételek listából</t>
   </si>
   <si>
     <t xml:space="preserve">TE_021</t>
@@ -504,23 +542,20 @@
   <si>
     <t xml:space="preserve">1. /admin URL megnyitása
 2. Jelszó beírása
-3. A Ételek szerkesztésének megjelenítése gomb
-Megnyomása
+3. Az Ételek szerkesztésének megjelenítése gomb megnyomása
 4. Új Étel hozzáadása gomb megnyomása
 5. Étel adatainak kitöltése
 6. Étel feltöltése gomb megnyomása
 7. Biztosan feltöltöd elfogadása
-8. Ételek gombra kattintás a navigációs
-Sávban.
+8. Ételek gombra kattintás a navigációs sávban.
 9. Egy étel kosárhoz adása a
 „Kosárba” gomb megnyomásával
-10. Kosár gomb megnyomása navigációs
-Sávban.
+10. Kosár gomb megnyomása navigációs sávban.
 11. Rendelési adatok kitöltése
 12. „Rendelés Küldése” gomb megnyomása
 13. /admin URL megnyitása
 14. A feltöltött étel kikeresése
-15. A Ételek szerkesztésének megjelenítése gomb
+15. Az Ételek szerkesztésének megjelenítése gomb megnyomása
 16. A feltöltött ételnél a törlés gomb megnyomása
 17. Biztosan törlöd elfogadása.</t>
   </si>
@@ -595,7 +630,7 @@
     <numFmt numFmtId="165" formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="166" formatCode="\$#,##0_);[RED]&quot;($&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -635,21 +670,45 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,20 +729,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF76FF03"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF1744"/>
+        <bgColor rgb="FFFF3D00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF1C99E0"/>
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF76FF03"/>
-        <bgColor rgb="FF00FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF3D00"/>
-        <bgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF1744"/>
       </patternFill>
     </fill>
   </fills>
@@ -870,7 +935,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -879,18 +944,38 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -903,7 +988,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -923,39 +1008,39 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -989,7 +1074,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFE6E6FF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF1744"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1161,8 +1246,8 @@
   </sheetPr>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1175,8 +1260,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="42.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="32.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="26.25"/>
   </cols>
   <sheetData>
@@ -1184,611 +1270,808 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="5"/>
+      <c r="D6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="60.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="5"/>
+      <c r="A7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="140.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="5"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="122.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="119.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="150.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" s="22" customFormat="true" ht="142.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="132.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="118" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="118" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="12"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="130.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="12"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="115.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="115.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="55.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="54.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="164.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="119.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8" t="s">
+      <c r="H22" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="K22" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" customFormat="false" ht="150.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" s="17" customFormat="true" ht="142.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" customFormat="false" ht="132.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" customFormat="false" ht="118" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" customFormat="false" ht="118" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="10"/>
-    </row>
-    <row r="16" customFormat="false" ht="130.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="10"/>
-    </row>
-    <row r="17" customFormat="false" ht="115.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="10"/>
-    </row>
-    <row r="18" customFormat="false" ht="115.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="9" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="198.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="10"/>
-    </row>
-    <row r="19" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="55.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="33.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="164.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" s="14" t="s">
+      <c r="L23" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="114.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-    </row>
-    <row r="23" customFormat="false" ht="198.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-    </row>
-    <row r="24" customFormat="false" ht="114.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
+      <c r="H24" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="95.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="309.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="3"/>
-      <c r="G28" s="17"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="3"/>
+      <c r="F29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="22"/>
+      <c r="F30" s="27"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="22"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="22"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="22"/>
+      <c r="F33" s="27"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="22"/>
+      <c r="F34" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="22">
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="G7:G18"/>
-    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="H8:H12"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="B12:B16"/>
@@ -1808,12 +2091,6 @@
     <mergeCell ref="F24:F26"/>
     <mergeCell ref="G24:G26"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="Név: Teszt Név &#10;Email: nev@example.com&#10;Telefonszám: 123123123"/>
-    <hyperlink ref="F9" r:id="rId2" display="Név: Teszt Bob &#10;Email: tesztbob@example.hu&#10;Telefonszám: 321321321"/>
-    <hyperlink ref="G22" r:id="rId3" display="Következő URL megnyitása:&#10;http://localhost:8080"/>
-    <hyperlink ref="G27" r:id="rId4" display="Következő URL megnyitása:&#10;http://localhost:8080"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>